<commit_message>
updated data layers table
</commit_message>
<xml_diff>
--- a/region2017/data_layers_table_wh.xlsx
+++ b/region2017/data_layers_table_wh.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eschemmel/Documents/github/WHI/region2017/layers_whi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eschemmel/Documents/github/WHI/region2017/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31840" yWindow="-1260" windowWidth="24040" windowHeight="12040" xr2:uid="{83F82C59-52CF-CE46-8AF1-F281A14C518B}"/>
+    <workbookView xWindow="-32520" yWindow="-740" windowWidth="24040" windowHeight="12040" xr2:uid="{83F82C59-52CF-CE46-8AF1-F281A14C518B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -305,9 +305,6 @@
     <t>DLNRDAR</t>
   </si>
   <si>
-    <t>commerical coastal pelagic fisheries catch</t>
-  </si>
-  <si>
     <t>fis_coast_pelagic_catch</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>Coastal pelagic fish catch (lbs) reported in the commercial fishery.</t>
   </si>
   <si>
-    <t>pelagic fisheries commerical catch</t>
-  </si>
-  <si>
     <t>fis_pelagic_catch</t>
   </si>
   <si>
@@ -329,9 +323,6 @@
     <t>Pelagic fish catch (lbs) reported in the commercial fishery.</t>
   </si>
   <si>
-    <t>sustainability of bottomfishery</t>
-  </si>
-  <si>
     <t>fis_sus</t>
   </si>
   <si>
@@ -695,9 +686,6 @@
     <t>A proxy for nutrient and chemical pollution measured as the percent of impervious surfaces per watershed with a maximum stresser level set at 10% of watershed area.</t>
   </si>
   <si>
-    <t>landbased source of pollution nitrogen</t>
-  </si>
-  <si>
     <t>po_lbsp_nosds</t>
   </si>
   <si>
@@ -851,9 +839,6 @@
     <t>t_env_sus_whi2018.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">The percent of nearhsore areas and priority watersheds protected in reference to Hawaii Sustainability Initatives (30 by 30 targets). This data may change as the State DLNR Division of Aquatic Resources develops the 30 by 30 initative. </t>
-  </si>
-  <si>
     <t>resident sentiment</t>
   </si>
   <si>
@@ -903,6 +888,21 @@
   </si>
   <si>
     <t>International Scientific Committee for Tuna and Tuna-like Species in the North Pacific Ocean (ISC), WCPFC</t>
+  </si>
+  <si>
+    <t>pelagic fisheries commercial catch</t>
+  </si>
+  <si>
+    <t>commercial coastal pelagic fisheries catch</t>
+  </si>
+  <si>
+    <t>sustainability of bottomfish fishery</t>
+  </si>
+  <si>
+    <t>land-based source of pollution nitrogen</t>
+  </si>
+  <si>
+    <t>The percent of nearhsore areas and priority watersheds protected.</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1258,7 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1772,16 +1772,16 @@
         <v>85</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>90</v>
@@ -1801,16 +1801,16 @@
         <v>85</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="G18" s="1">
         <v>2012</v>
@@ -1836,16 +1836,16 @@
         <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="H19" s="1">
         <v>2018</v>
@@ -1854,10 +1854,10 @@
         <v>37</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1868,16 +1868,16 @@
         <v>85</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G20" s="1">
         <v>2014</v>
@@ -1886,16 +1886,16 @@
         <v>2017</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1906,16 +1906,16 @@
         <v>85</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H21" s="1">
         <v>2017</v>
@@ -1924,10 +1924,10 @@
         <v>37</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1935,19 +1935,19 @@
         <v>84</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="G22" s="1">
         <v>2017</v>
@@ -1956,10 +1956,10 @@
         <v>2017</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1967,25 +1967,25 @@
         <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="I23" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1993,19 +1993,19 @@
         <v>84</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G24" s="1">
         <v>2007</v>
@@ -2014,13 +2014,13 @@
         <v>2011</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2028,19 +2028,19 @@
         <v>84</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="G25" s="1">
         <v>2017</v>
@@ -2049,10 +2049,10 @@
         <v>2017</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -2060,19 +2060,19 @@
         <v>84</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="G26" s="1">
         <v>2002</v>
@@ -2081,33 +2081,33 @@
         <v>2011</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="G27" s="1">
         <v>2005</v>
@@ -2116,62 +2116,62 @@
         <v>2013</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="I28" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="G29" s="1">
         <v>2005</v>
@@ -2180,524 +2180,524 @@
         <v>2013</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="J30" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="J31" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="J32" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="J33" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="I34" s="1" t="s">
+      <c r="L34" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="K35" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="J36" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="J37" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="I38" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>218</v>
-      </c>
       <c r="I39" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>222</v>
-      </c>
       <c r="I40" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="J41" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="K43" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="K43" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>248</v>
-      </c>
       <c r="K45" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="J47" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="K47" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="K48" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>269</v>
       </c>
       <c r="G49" s="1">
         <v>2012</v>
@@ -2706,30 +2706,30 @@
         <v>2016</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>275</v>
+        <v>292</v>
       </c>
       <c r="G50" s="1">
         <v>2011</v>
@@ -2738,30 +2738,30 @@
         <v>2016</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="G51" s="1">
         <v>2011</v>
@@ -2770,33 +2770,33 @@
         <v>2015</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="G52" s="1">
         <v>2012</v>
@@ -2805,27 +2805,27 @@
         <v>2016</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="G53" s="1">
         <v>2011</v>
@@ -2834,10 +2834,10 @@
         <v>2016</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>